<commit_message>
select upd && corrections
</commit_message>
<xml_diff>
--- a/backend/static/report.xlsx
+++ b/backend/static/report.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="13"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Титульный" sheetId="1" state="visible" r:id="rId3"/>
@@ -181,7 +181,7 @@
     <t xml:space="preserve">4. Статус объекта (памятник архитектуры, исторический памятник и т.д.) </t>
   </si>
   <si>
-    <t xml:space="preserve">{Статус объекта} || Не устанавливается</t>
+    <t xml:space="preserve">{Статус объекта} || Не устанавливался</t>
   </si>
   <si>
     <t xml:space="preserve">5. Тип проекта объекта</t>
@@ -1648,9 +1648,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>115200</xdr:colOff>
+      <xdr:colOff>114840</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>95400</xdr:rowOff>
+      <xdr:rowOff>95040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1664,7 +1664,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="281160" y="66240"/>
-          <a:ext cx="1347840" cy="568440"/>
+          <a:ext cx="1347480" cy="568080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1691,9 +1691,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>164520</xdr:colOff>
+      <xdr:colOff>164160</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>110520</xdr:rowOff>
+      <xdr:rowOff>110160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1707,7 +1707,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="510120" y="81360"/>
-          <a:ext cx="1347840" cy="568440"/>
+          <a:ext cx="1347480" cy="568080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1734,9 +1734,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>35</xdr:col>
-      <xdr:colOff>114840</xdr:colOff>
+      <xdr:colOff>114480</xdr:colOff>
       <xdr:row>56</xdr:row>
-      <xdr:rowOff>135720</xdr:rowOff>
+      <xdr:rowOff>135360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1750,7 +1750,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5803920" y="10002240"/>
-          <a:ext cx="676800" cy="284040"/>
+          <a:ext cx="676440" cy="283680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -12354,7 +12354,7 @@
   </sheetPr>
   <dimension ref="A1:BW1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -26156,8 +26156,8 @@
   </sheetPr>
   <dimension ref="A1:BW1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AV7" activeCellId="0" sqref="AV7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="U16" activeCellId="0" sqref="U16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.55078125" defaultRowHeight="14.15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>